<commit_message>
data revision... about_details not working
</commit_message>
<xml_diff>
--- a/meta/faq.xlsx
+++ b/meta/faq.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reiter\Dropbox\Data Explorer 2.0\meta-to-wcde\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clreiter\Dropbox\Data Explorer 2.0\meta-to-wcde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E16AB48-E8CB-4366-BFE8-DFA6B5838911}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="faq" sheetId="1" r:id="rId1"/>
@@ -324,19 +323,19 @@
     <t>Why is the data in the Data Explorer slightly &lt;strong&gt;different from the data published&lt;/strong&gt; in &lt;a href="https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries"&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt;?</t>
   </si>
   <si>
-    <t xml:space="preserve">Due to insufficient data on sub-categories for post-secondary education, the categories 'Short Post-Secondary', 'Bachelor' and 'Master and higher' are only available for EU-28 countries from 2015 onwards. </t>
-  </si>
-  <si>
     <t>Is there also information on &lt;strong&gt;immigration and emigration&lt;/strong&gt; available?</t>
   </si>
   <si>
     <t>Why do I get the following warning when I submit my selection: 'Your selection includes at least &lt;strong&gt;one country with limited base year data&lt;/strong&gt; on educational attainment. Please consult the FAQ for more information.'?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to insufficient data on sub-categories for post-secondary education, the categories 'Short Post-Secondary', 'Bachelor' and 'Master and higher' are only available for 59 countries from 2015 onwards. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -973,23 +972,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1025,23 +1007,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1217,15 +1182,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1382,7 +1345,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>44</v>
@@ -1429,7 +1392,7 @@
         <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1481,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
new data and almost final suggestions
</commit_message>
<xml_diff>
--- a/meta/faq.xlsx
+++ b/meta/faq.xlsx
@@ -287,12 +287,6 @@
     <t>Why is there a &lt;strong&gt;break in time series&lt;/strong&gt; between 2010 and 2015 for many &lt;strong&gt;regions&lt;/strong&gt; and indicators?</t>
   </si>
   <si>
-    <t>The main reason is that the reconstruction uses a different base-year dataset. Furthermore, the methodology was slightly modified, making usage of validated historical datasets. For more information see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/PDF/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al. 2019&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Education categories used in the projections are in line with selected UNESCO's &lt;a href='http://www.uis.unesco.org/Education/Pages/international-standard-classification-of-education.aspx'&gt;International Standard Classification of Education (ISCED 2011) categories&lt;/a&gt;. For details on WIC categories, see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/PDF/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al., 2019, VID WP 02/2019&lt;/a&gt; or the Education Definitions tab.</t>
-  </si>
-  <si>
     <t>The projection data come from population projections carried out by researchers at WIC. They are based on several data collection excercises for the base-year data and historical reconstruction to 1950. The research also uses largely the data produced by &lt;a href='http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm'&gt;World Population Prospects: The 2017 revision&lt;/a&gt; by the United Nations Population Division (2015 base-year population by age and sex and estimates for 1950-2010, and information about fertility, mortality and migration and related indicators for 1950-2015). The data are explained in two publications: &lt;a href='https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries'&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt; and &lt;a href='https://global.oup.com/academic/product/world-population-and-human-capital-in-the-twenty-first-century-9780198703167?cc=at&amp;lang=en'&gt;Lutz, Butz, and K.C. (Eds.) (2014)&lt;/a&gt;.</t>
   </si>
   <si>
@@ -330,6 +324,12 @@
   </si>
   <si>
     <t xml:space="preserve">Due to insufficient data on sub-categories for post-secondary education, the categories 'Short Post-Secondary', 'Bachelor' and 'Master and higher' are only available for 59 countries from 2015 onwards. </t>
+  </si>
+  <si>
+    <t>Education categories used in the projections are in line with selected UNESCO's &lt;a href='http://www.uis.unesco.org/Education/Pages/international-standard-classification-of-education.aspx'&gt;International Standard Classification of Education (ISCED 2011) categories&lt;/a&gt;. For details on WIC categories, see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al., 2019, VID WP 02/2019&lt;/a&gt; or the Education Definitions tab.</t>
+  </si>
+  <si>
+    <t>The main reason is that the reconstruction uses a different base-year dataset. Furthermore, the methodology was slightly modified, making usage of validated historical datasets. For more information see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al. 2019&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>44</v>
@@ -1381,7 +1381,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1389,10 +1389,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1433,7 +1433,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>48</v>
@@ -1444,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>57</v>
@@ -1455,7 +1455,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>35</v>
@@ -1466,7 +1466,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>49</v>
@@ -1477,10 +1477,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1488,10 +1488,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>58</v>
@@ -1532,7 +1532,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
faq revised to do generated
</commit_message>
<xml_diff>
--- a/meta/faq.xlsx
+++ b/meta/faq.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abel\Documents\GitHub\wcde-shiny\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyildiz\Dropbox\PC\Documents\GitHub\fume-shiny\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E655BC-1E9A-4D13-8DC3-463A72971952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="faq" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>category</t>
   </si>
@@ -105,9 +106,6 @@
     <t>Which and how many &lt;strong&gt;scenarios&lt;/strong&gt; are included in the WIC Data Explorer?</t>
   </si>
   <si>
-    <t>The &lt;a href='http://www.wittgensteincentre.org/'&gt;Wittgenstein Centre for Demography and Global Human Capital (WIC)&lt;/a&gt; is based in Vienna and Laxenburg, Austria. It is a collaboration between the &lt;a href='http://www.iiasa.ac.at/'&gt;International Institute for Applied Systems Analysis (IIASA&lt;/a&gt;), the &lt;a href='http://www.oeaw.ac.at/vid/'&gt;Vienna Institute of Demography of the Austrian Academy of Sciences (VID/OEAW)&lt;/a&gt;, and the &lt;a href='http://wu.ac.at/'&gt;Vienna University of Economics and Business (WU)&lt;/a&gt;. Its aim is to be a world leader in the advancement of demographic methods and their application to the analysis of human capital and population dynamics by combining the three partner organizations' strengths in the fields of demography, human capital formation, and analysis of the returns to education.</t>
-  </si>
-  <si>
     <t>Yes, webmasters can place links to the WIC Data Explorer without  special permission. Nevertheless, we would appreciate &lt;a href='mailto:data@wittgensteincentre.org'&gt;notification&lt;/a&gt; if you do so.</t>
   </si>
   <si>
@@ -153,41 +151,89 @@
     <t>It is possible to select the total population or five year age groups from 0 to 4 until 95 to 99 as well as the age group 100+ (the maximum age group considered).</t>
   </si>
   <si>
-    <t>For 16 countries it was not possible to obtain data on educational attainment for the base year. Hence, approximations based on regional averages were computed instead. Data for these countries should be used with utmost care. The countries in question are the following: Antigua and Barbuda, Barbados, Brunei Darussalem, Channel Islands, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara.</t>
-  </si>
-  <si>
     <t xml:space="preserve">PDF reports are available for all 201 countries, with tables of detailed results of projections for each of the EU-28 countries, and tables with chosen results of projections for all of the other countries in the world. </t>
   </si>
   <si>
     <t>For which countries are &lt;strong&gt;PDFs with additional information&lt;/strong&gt; available?</t>
   </si>
   <si>
-    <t>Five different scenarios from the Wittgenstein Global Human Capital projections are included in the WIC Data Explorer, following the Shared Socioeconomic Pathways (SSPs). For the detailed assumptions for every scenario see the Scenario Definitions tab.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of countries with data on educational attainement has been increased to 185 (from 171 in Version 1.2). We have updated the education data with the most recent valid datasets. Whenever possible, we have also disaggregated the post-secondary education category in more categories following ISCED 11. Furthermore, the reconstruction goes back to 1950 (instead of 1970 in Version 1.2). </t>
-  </si>
-  <si>
-    <t>Due to methodological constraints, only countries with a population of more than 100,000 people in 2015 are currently considered in the database (the Seychelles is the only exception).</t>
-  </si>
-  <si>
-    <t>The WIC Data Explorer currently includes data on the following topics for 201 countries of the world: total population and population growth, population ageing, education, fertility, mortality, and migration. Not all indicators are available in every scenario, by education, and/or at all geographical scales.</t>
-  </si>
-  <si>
-    <t>The projections by education until 2100 are based on collected census and survey data for the base year (around 2015). They follow different what-if scenarios to show the development over time if certain criteria are met. For more information see the Scenario Definitions tab.</t>
-  </si>
-  <si>
-    <t>The copyright of all data provided in the WIC Data Explorer belongs to the Wittgenstein Centre for Demography and Global Human Capital and its researchers. Data can be used for personal calculations and publications and should be  referenced as follows: 'Source: Wittgenstein Centre for Demography and Global Human Capital (WIC) Wittgenstein Centre Data Explorer. Version 2.0 2018'</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data selection in WIC Data Explorer is done in four steps: (1) Select your indicator; (2) Select the geography by choosing countries and/or regions; (3) Choose the preferred sex and age categories; (4) Choose the  scenarios and years. Then click the 'View Data' button to view your selection. Furthermore, in all fields of the WIC Data Explorer you can type or click to make your selection and to get suggestions. You can also use the backspace command to remove entries from your selection. </t>
   </si>
   <si>
-    <t>201 countries are included in the WIC Data Explorer. However, for 16 countries (Antigua and Barbuda, Barbados, Brunei Darussalem, Channel Islands, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara), we did not find education data. Hence, regional averages or similar countries were used instead and we recommend careful use of their data. For those countries, we do not reconstruct back to 1950. World regions and sub regions are adopted from the United Nations (UN). For more information on the UN definitions click &lt;a href='https://unstats.un.org/unsd/methodology/m49/'&gt;here&lt;/a&gt;.</t>
+    <t xml:space="preserve">Why are &lt;strong&gt;Age-specific Fertility Rates by Education&lt;/strong&gt; and &lt;strong&gt;Total Fertility Rates by Education&lt;/strong&gt; in many cases equal for different education categories? </t>
+  </si>
+  <si>
+    <t>Due to methodological reasons, education categories are aggregated whenever their share in total population is below a certain threshold.</t>
+  </si>
+  <si>
+    <t>This is due to methodological constraints. As a result of different weights for different countries, regional aggregates of education-specific total fertility rates tend to show unsteady results.</t>
+  </si>
+  <si>
+    <t>In the bottom right of the WIC Data Explorer you will find the download button for your current data selection. Choose the WIC Graphic Explorer, if you want to download PDFs or PNGs of maps, pyramids, and education stack charts.</t>
+  </si>
+  <si>
+    <t>Why are &lt;strong&gt;regional aggregates&lt;/strong&gt; for the indicator &lt;strong&gt;Total Fertility Rate by Education&lt;/strong&gt; very volatile, while country results look smooth?</t>
+  </si>
+  <si>
+    <t>Why do I get the following message in the table when I submit my selection: '&lt;strong&gt;No data available&lt;/strong&gt; in table'?</t>
+  </si>
+  <si>
+    <t>Is there also information on &lt;strong&gt;immigration and emigration&lt;/strong&gt; available?</t>
+  </si>
+  <si>
+    <t>Why do I get the following warning when I submit my selection: 'Your selection includes at least &lt;strong&gt;one country with limited base year data&lt;/strong&gt; on educational attainment. Please consult the FAQ for more information.'?</t>
+  </si>
+  <si>
+    <t>Education categories used in the projections are in line with selected UNESCO's &lt;a href='http://www.uis.unesco.org/Education/Pages/international-standard-classification-of-education.aspx'&gt;International Standard Classification of Education (ISCED 2011) categories&lt;/a&gt;. For details on WIC categories, see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al., 2019, VID WP 02/2019&lt;/a&gt; or the Education Definitions tab.</t>
+  </si>
+  <si>
+    <t>The &lt;a href='http://www.wittgensteincentre.org/'&gt;Wittgenstein Centre for Demography and Global Human Capital (WIC)&lt;/a&gt; is based in Vienna and Laxenburg, Austria. It is a collaboration between the &lt;a href='http://www.iiasa.ac.at/'&gt;International Institute for Applied Systems Analysis (IIASA&lt;/a&gt;), the &lt;a href='http://www.oeaw.ac.at/vid/'&gt;Vienna Institute of Demography of the Austrian Academy of Sciences (VID/OEAW)&lt;/a&gt;, and the &lt;a href='http://univie.ac.at/'&gt;University of Vienna&lt;/a&gt;. Its aim is to be a world leader in the advancement of demographic methods and their application to the analysis of human capital and population dynamics by combining the three partner organizations' strengths in the fields of demography, human capital formation, and analysis of the returns to education.</t>
+  </si>
+  <si>
+    <t>The WIC Data Explorer currently includes data on the following topics for 200 countries of the world: total population and population growth, population ageing, education, fertility, mortality, and migration. Not all indicators are available in every scenario, by education, and/or at all geographical scales.</t>
+  </si>
+  <si>
+    <t>The projection data come from population projections carried out by researchers at WIC. They are based on several data collection excercises for the base-year data and historical reconstruction to 1950. The research also uses largely the data produced by &lt;a href='http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm'&gt;World Population Prospects: The 2022 revision&lt;/a&gt; by the United Nations Population Division (2020 base-year population by age and sex and estimates for 1950-2015, and information about fertility, mortality and migration and related indicators for 1950-2020). The data are explained in two publications: &lt;a href='https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries'&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt; and &lt;a href='https://global.oup.com/academic/product/world-population-and-human-capital-in-the-twenty-first-century-9780198703167?cc=at&amp;lang=en'&gt;Lutz, Butz, and K.C. (Eds.) (2014)&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>The projections by education until 2100 are based on collected census and survey data for the base year (around 2020). They follow different what-if scenarios to show the development over time if certain criteria are met. For more information see the Scenario Definitions tab.</t>
+  </si>
+  <si>
+    <t>The copyright of all data provided in the WIC Data Explorer belongs to the Wittgenstein Centre for Demography and Global Human Capital and its researchers. Data can be used for personal calculations and publications and should be  referenced as follows: 'Source: Wittgenstein Centre for Demography and Global Human Capital (WIC) Wittgenstein Centre Data Explorer. Version 3.0 2023'</t>
+  </si>
+  <si>
+    <t>What is the &lt;strong&gt;reference time&lt;/strong&gt; for the WIC data?</t>
+  </si>
+  <si>
+    <t>The reference time for WIC data is 1st of January of the year in question.</t>
+  </si>
+  <si>
+    <t>For 15 countries it was not possible to obtain data on educational attainment for the base year. Hence, approximations based on regional averages were computed instead. Data for these countries should be used with utmost care. The countries in question are the following: Antigua and Barbuda, Barbados, Brunei Darussalem, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara.</t>
+  </si>
+  <si>
+    <t>Due to methodological constraints, only countries with a population of more than 80,000 people in 2020 are currently considered in the database (the Seychelles is the only exception).</t>
+  </si>
+  <si>
+    <t>The reconstruction of population by levels of educational attainment from 1950 to 2020 will be made available in 2024.</t>
+  </si>
+  <si>
+    <t>Why is there no data for the period &lt;strong&gt;before 2020&lt;/strong&gt;?</t>
+  </si>
+  <si>
+    <t>Why is the &lt;strong&gt;8 education categories&lt;/strong&gt; choice not available for this version?</t>
+  </si>
+  <si>
+    <t>In this version we decided to consider only 6 education categories.</t>
+  </si>
+  <si>
+    <t>200 countries are included in the WIC Data Explorer. However, for 15 countries (Antigua and Barbuda, Barbados, Brunei Darussalem, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara), we did not find education data. Hence, regional averages or similar countries were used instead and we recommend careful use of their data. World regions and sub regions are adopted from the United Nations (UN). For more information on the UN definitions click &lt;a href='https://unstats.un.org/unsd/methodology/m49/'&gt;here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Seven different scenarios from the Wittgenstein Global Human Capital projections are included in the WIC Data Explorer, following the Shared Socioeconomic Pathways (SSPs). For the detailed assumptions for every scenario see the Scenario Definitions tab.</t>
   </si>
   <si>
     <r>
-      <t>Currently data are included from 1950 until 2100. The base year for the projections is 2015. Stock estimates (e.g. population size) refer to 1</t>
+      <t>Currently data are included from 2020 until 2100. The base year for the projections is 2020. Stock estimates (e.g. population size) refer to 1</t>
     </r>
     <r>
       <rPr>
@@ -208,7 +254,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of July of the year in question. Period estimates (e.g. total fertility rates) refer to the period between the 1</t>
+      <t xml:space="preserve"> of January of the year in question. Period estimates (e.g. total fertility rates) refer to the period between the 1</t>
     </r>
     <r>
       <rPr>
@@ -229,7 +275,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of July of the starting year and 30</t>
+      <t xml:space="preserve"> of January of the starting year and 31</t>
     </r>
     <r>
       <rPr>
@@ -250,92 +296,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of June of the ending year of the period in question.</t>
+      <t xml:space="preserve"> of December of the ending year of the period in question.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Yes, data on immigration on emigration is available upon request. The assumptions used are based on &lt;a href='https://guyabel.com/publication/global-migration-estimates-by-gender/'&gt;Abel, 2017&lt;/a&gt;, from where you can obtain in- and outflow data from 1960 to 2015. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is due to later data adjustments in the course of validating the Data Explorer 2.0, resulting in minor changes to the projection results. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why are &lt;strong&gt;Age-specific Fertility Rates by Education&lt;/strong&gt; and &lt;strong&gt;Total Fertility Rates by Education&lt;/strong&gt; in many cases equal for different education categories? </t>
-  </si>
-  <si>
-    <t>Due to methodological reasons, education categories are aggregated whenever their share in total population is below a certain threshold.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While the reconstruction of population by levels of educational attainment from 1950 to 2015 covers 185 countries, population projections include 201 countries. Hence, proxy data for the missing countries have to be used to calculate regional aggregates, resulting in minor breaks in time series. </t>
-  </si>
-  <si>
-    <t>This is due to methodological constraints. As a result of different weights for different countries, regional aggregates of education-specific total fertility rates tend to show unsteady results.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due to methodological reasons slightly different calculations are used for the historical reconstruction (based on 6 education categories) and the projections (based on 8 education categories) of this indicator. </t>
-  </si>
-  <si>
-    <t>In the bottom right of the WIC Data Explorer you will find the download button for your current data selection. Choose the WIC Graphic Explorer, if you want to download PDFs or PNGs of maps, pyramids, and education stack charts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why is there a break in time series between 2010 and 2015 for &lt;strong&gt;Mean Years of Schooling&lt;/strong&gt; for some countries? </t>
-  </si>
-  <si>
-    <t>Why is there a &lt;strong&gt;break in time series&lt;/strong&gt; between 2010 and 2015 for many &lt;strong&gt;regions&lt;/strong&gt; and indicators?</t>
-  </si>
-  <si>
-    <t>The projection data come from population projections carried out by researchers at WIC. They are based on several data collection excercises for the base-year data and historical reconstruction to 1950. The research also uses largely the data produced by &lt;a href='http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm'&gt;World Population Prospects: The 2017 revision&lt;/a&gt; by the United Nations Population Division (2015 base-year population by age and sex and estimates for 1950-2010, and information about fertility, mortality and migration and related indicators for 1950-2015). The data are explained in two publications: &lt;a href='https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries'&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt; and &lt;a href='https://global.oup.com/academic/product/world-population-and-human-capital-in-the-twenty-first-century-9780198703167?cc=at&amp;lang=en'&gt;Lutz, Butz, and K.C. (Eds.) (2014)&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Why are &lt;strong&gt;regional aggregates&lt;/strong&gt; for the indicator &lt;strong&gt;Total Fertility Rate by Education&lt;/strong&gt; very volatile, while country results look smooth?</t>
-  </si>
-  <si>
-    <t>Why do I get the following message in the table when I submit my selection: '&lt;strong&gt;No data available&lt;/strong&gt; in table'?</t>
-  </si>
-  <si>
-    <t>Why is the &lt;strong&gt;8 education categories&lt;/strong&gt; choice not available for all countries and all years?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UN Population Division, World Population Prospects 2017 data was obtained through the R package 'wpp2017' which displays slightly different values than the download files. </t>
-  </si>
-  <si>
-    <t>Why are &lt;strong&gt;SSP4 and 5 not available&lt;/strong&gt; anymore in Version 2.0?</t>
-  </si>
-  <si>
-    <t>Why is the &lt;strong&gt;reconstructed data&lt;/strong&gt; from 1970 to 2010 different from Version 1.2?</t>
-  </si>
-  <si>
-    <t>What is &lt;strong&gt;new compared to Version 1.2&lt;/strong&gt;?</t>
-  </si>
-  <si>
-    <t>Why is data referenced to &lt;a href="http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm"&gt;&lt;strong&gt;UN Population Division, World Population Prospects 2017&lt;/strong&gt;&lt;/a&gt; slightly different from what I find in UN World Population Prospects 2017 &lt;a href="https://population.un.org/wpp/Download/Standard/Population/"&gt;download files&lt;/a&gt;?</t>
-  </si>
-  <si>
-    <t>Why is the data in the Data Explorer slightly &lt;strong&gt;different from the data published&lt;/strong&gt; in &lt;a href="https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries"&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt;?</t>
-  </si>
-  <si>
-    <t>Is there also information on &lt;strong&gt;immigration and emigration&lt;/strong&gt; available?</t>
-  </si>
-  <si>
-    <t>Why do I get the following warning when I submit my selection: 'Your selection includes at least &lt;strong&gt;one country with limited base year data&lt;/strong&gt; on educational attainment. Please consult the FAQ for more information.'?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due to insufficient data on sub-categories for post-secondary education, the categories 'Short Post-Secondary', 'Bachelor' and 'Master and higher' are only available for 59 countries from 2015 onwards. </t>
-  </si>
-  <si>
-    <t>Education categories used in the projections are in line with selected UNESCO's &lt;a href='http://www.uis.unesco.org/Education/Pages/international-standard-classification-of-education.aspx'&gt;International Standard Classification of Education (ISCED 2011) categories&lt;/a&gt;. For details on WIC categories, see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al., 2019, VID WP 02/2019&lt;/a&gt; or the Education Definitions tab.</t>
-  </si>
-  <si>
-    <t>The main reason is that the reconstruction uses a different base-year dataset. Furthermore, the methodology was slightly modified, making usage of validated historical datasets. For more information see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al. 2019&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>SSP4 and SSP5 were finalized in 2020 (&lt;a href = 'http://pure.iiasa.ac.at/id/eprint/16710/1/WP-20-016.pdf'&gt;link&lt;/a&gt;), the results for population and mean years of schooling can be downloaded directly &lt;a href = 'http://pure.iiasa.ac.at/id/eprint/17550/1/Global population and human capital projections.zip'&gt;here&lt;/a&gt;.</t>
+    <t xml:space="preserve">Yes, data on immigration on emigration is available upon request. The assumptions used are based on &lt;a href='https://guyabel.com//publication//bilateral-migration-flow-sex//'&gt;Abel, 2022&lt;/a&gt;, from where you can obtain in- and outflow data from 1990 to 2020. </t>
+  </si>
+  <si>
+    <t>What is &lt;strong&gt;new compared to Version 2&lt;/strong&gt;?</t>
+  </si>
+  <si>
+    <t>The Version 3 update is the most comprehensive since 2013, extending beyond updating the base year to 2020. Short-term assumptions (up to 2030) have been occasionally updated, while assumptions for 2050 and 2100 remain largely unchanged since they were based on comprehensive analyses and expert input. However, the trend component of the assumptions has been modified based on recent observations. Modeling methodology, fertility, migration, and education have also been modified. Education-specific fertility levels have been updated with new estimates, and education differentials in mortality are now country- and region-specific rather than being normalized to a single level by gender. Also, education-specific migration rates are implemented in the projection model for the first time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -972,6 +949,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1007,6 +1001,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1182,14 +1193,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1229,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,7 +1251,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,7 +1262,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1284,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1295,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1303,10 +1314,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1314,32 +1325,32 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1347,21 +1358,21 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1369,32 +1380,32 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>78</v>
+      <c r="C18" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1402,10 +1413,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1413,10 +1424,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1424,10 +1435,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1435,10 +1446,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1446,10 +1457,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1457,10 +1468,10 @@
         <v>8</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1468,10 +1479,10 @@
         <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1482,18 +1493,18 @@
         <v>72</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>70</v>
+      <c r="B27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1501,54 +1512,54 @@
         <v>8</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1556,10 +1567,10 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1567,10 +1578,10 @@
         <v>14</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1578,61 +1589,17 @@
         <v>14</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B39" s="5"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
+      <c r="C43" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes as discusssed with Anne
</commit_message>
<xml_diff>
--- a/meta/faq.xlsx
+++ b/meta/faq.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyildiz\Dropbox\PC\Documents\GitHub\fume-shiny\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyildiz\Dropbox\PC\Documents\GitHub\wcde-shiny-2023\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E655BC-1E9A-4D13-8DC3-463A72971952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFE4034-A3B0-4C15-A5D1-3C5A2AA0D5D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>category</t>
   </si>
@@ -151,12 +151,6 @@
     <t>It is possible to select the total population or five year age groups from 0 to 4 until 95 to 99 as well as the age group 100+ (the maximum age group considered).</t>
   </si>
   <si>
-    <t xml:space="preserve">PDF reports are available for all 201 countries, with tables of detailed results of projections for each of the EU-28 countries, and tables with chosen results of projections for all of the other countries in the world. </t>
-  </si>
-  <si>
-    <t>For which countries are &lt;strong&gt;PDFs with additional information&lt;/strong&gt; available?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data selection in WIC Data Explorer is done in four steps: (1) Select your indicator; (2) Select the geography by choosing countries and/or regions; (3) Choose the preferred sex and age categories; (4) Choose the  scenarios and years. Then click the 'View Data' button to view your selection. Furthermore, in all fields of the WIC Data Explorer you can type or click to make your selection and to get suggestions. You can also use the backspace command to remove entries from your selection. </t>
   </si>
   <si>
@@ -178,55 +172,25 @@
     <t>Why do I get the following message in the table when I submit my selection: '&lt;strong&gt;No data available&lt;/strong&gt; in table'?</t>
   </si>
   <si>
-    <t>Is there also information on &lt;strong&gt;immigration and emigration&lt;/strong&gt; available?</t>
-  </si>
-  <si>
     <t>Why do I get the following warning when I submit my selection: 'Your selection includes at least &lt;strong&gt;one country with limited base year data&lt;/strong&gt; on educational attainment. Please consult the FAQ for more information.'?</t>
   </si>
   <si>
-    <t>Education categories used in the projections are in line with selected UNESCO's &lt;a href='http://www.uis.unesco.org/Education/Pages/international-standard-classification-of-education.aspx'&gt;International Standard Classification of Education (ISCED 2011) categories&lt;/a&gt;. For details on WIC categories, see &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al., 2019, VID WP 02/2019&lt;/a&gt; or the Education Definitions tab.</t>
-  </si>
-  <si>
-    <t>The &lt;a href='http://www.wittgensteincentre.org/'&gt;Wittgenstein Centre for Demography and Global Human Capital (WIC)&lt;/a&gt; is based in Vienna and Laxenburg, Austria. It is a collaboration between the &lt;a href='http://www.iiasa.ac.at/'&gt;International Institute for Applied Systems Analysis (IIASA&lt;/a&gt;), the &lt;a href='http://www.oeaw.ac.at/vid/'&gt;Vienna Institute of Demography of the Austrian Academy of Sciences (VID/OEAW)&lt;/a&gt;, and the &lt;a href='http://univie.ac.at/'&gt;University of Vienna&lt;/a&gt;. Its aim is to be a world leader in the advancement of demographic methods and their application to the analysis of human capital and population dynamics by combining the three partner organizations' strengths in the fields of demography, human capital formation, and analysis of the returns to education.</t>
-  </si>
-  <si>
     <t>The WIC Data Explorer currently includes data on the following topics for 200 countries of the world: total population and population growth, population ageing, education, fertility, mortality, and migration. Not all indicators are available in every scenario, by education, and/or at all geographical scales.</t>
   </si>
   <si>
-    <t>The projection data come from population projections carried out by researchers at WIC. They are based on several data collection excercises for the base-year data and historical reconstruction to 1950. The research also uses largely the data produced by &lt;a href='http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm'&gt;World Population Prospects: The 2022 revision&lt;/a&gt; by the United Nations Population Division (2020 base-year population by age and sex and estimates for 1950-2015, and information about fertility, mortality and migration and related indicators for 1950-2020). The data are explained in two publications: &lt;a href='https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries'&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt; and &lt;a href='https://global.oup.com/academic/product/world-population-and-human-capital-in-the-twenty-first-century-9780198703167?cc=at&amp;lang=en'&gt;Lutz, Butz, and K.C. (Eds.) (2014)&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>The projections by education until 2100 are based on collected census and survey data for the base year (around 2020). They follow different what-if scenarios to show the development over time if certain criteria are met. For more information see the Scenario Definitions tab.</t>
   </si>
   <si>
-    <t>The copyright of all data provided in the WIC Data Explorer belongs to the Wittgenstein Centre for Demography and Global Human Capital and its researchers. Data can be used for personal calculations and publications and should be  referenced as follows: 'Source: Wittgenstein Centre for Demography and Global Human Capital (WIC) Wittgenstein Centre Data Explorer. Version 3.0 2023'</t>
-  </si>
-  <si>
     <t>What is the &lt;strong&gt;reference time&lt;/strong&gt; for the WIC data?</t>
   </si>
   <si>
     <t>The reference time for WIC data is 1st of January of the year in question.</t>
   </si>
   <si>
-    <t>For 15 countries it was not possible to obtain data on educational attainment for the base year. Hence, approximations based on regional averages were computed instead. Data for these countries should be used with utmost care. The countries in question are the following: Antigua and Barbuda, Barbados, Brunei Darussalem, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara.</t>
-  </si>
-  <si>
-    <t>Due to methodological constraints, only countries with a population of more than 80,000 people in 2020 are currently considered in the database (the Seychelles is the only exception).</t>
-  </si>
-  <si>
     <t>The reconstruction of population by levels of educational attainment from 1950 to 2020 will be made available in 2024.</t>
   </si>
   <si>
     <t>Why is there no data for the period &lt;strong&gt;before 2020&lt;/strong&gt;?</t>
-  </si>
-  <si>
-    <t>Why is the &lt;strong&gt;8 education categories&lt;/strong&gt; choice not available for this version?</t>
-  </si>
-  <si>
-    <t>In this version we decided to consider only 6 education categories.</t>
-  </si>
-  <si>
-    <t>200 countries are included in the WIC Data Explorer. However, for 15 countries (Antigua and Barbuda, Barbados, Brunei Darussalem, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara), we did not find education data. Hence, regional averages or similar countries were used instead and we recommend careful use of their data. World regions and sub regions are adopted from the United Nations (UN). For more information on the UN definitions click &lt;a href='https://unstats.un.org/unsd/methodology/m49/'&gt;here&lt;/a&gt;.</t>
   </si>
   <si>
     <t>Seven different scenarios from the Wittgenstein Global Human Capital projections are included in the WIC Data Explorer, following the Shared Socioeconomic Pathways (SSPs). For the detailed assumptions for every scenario see the Scenario Definitions tab.</t>
@@ -300,13 +264,31 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Yes, data on immigration on emigration is available upon request. The assumptions used are based on &lt;a href='https://guyabel.com//publication//bilateral-migration-flow-sex//'&gt;Abel, 2022&lt;/a&gt;, from where you can obtain in- and outflow data from 1990 to 2020. </t>
-  </si>
-  <si>
     <t>What is &lt;strong&gt;new compared to Version 2&lt;/strong&gt;?</t>
   </si>
   <si>
     <t>The Version 3 update is the most comprehensive since 2013, extending beyond updating the base year to 2020. Short-term assumptions (up to 2030) have been occasionally updated, while assumptions for 2050 and 2100 remain largely unchanged since they were based on comprehensive analyses and expert input. However, the trend component of the assumptions has been modified based on recent observations. Modeling methodology, fertility, migration, and education have also been modified. Education-specific fertility levels have been updated with new estimates, and education differentials in mortality are now country- and region-specific rather than being normalized to a single level by gender. Also, education-specific migration rates are implemented in the projection model for the first time.</t>
+  </si>
+  <si>
+    <t>The &lt;a href='http://www.wittgensteincentre.org/'&gt;Wittgenstein Centre for Demography and Global Human Capital (WIC)&lt;/a&gt; is based in Vienna and Laxenburg, Austria. It is a collaboration between the &lt;a href='http://www.iiasa.ac.at/'&gt;International Institute for Applied Systems Analysis (IIASA&lt;/a&gt;), the &lt;a href='http://www.oeaw.ac.at/vid/'&gt;Vienna Institute of Demography of the Austrian Academy of Sciences (VID/OEAW)&lt;/a&gt;, and the &lt;a href='http://univie.ac.at/'&gt;University of Vienna&lt;/a&gt;. The aim of the Wittgenstein Centre is to advance demographic methods and their application in analyzing human capital and population dynamics by leveraging the strengths of the three partner organizations in the fields of demography, human capital formation, and the analysis of returns to education.</t>
+  </si>
+  <si>
+    <t>The copyright of all data provided in the WIC Data Explorer belongs to the Wittgenstein Centre for Demography and Global Human Capital and its researchers. Data can be used for personal calculations and publications and should be referenced as follows: 'Source: Wittgenstein Centre for Demography and Global Human Capital (WIC) Wittgenstein Centre Data Explorer. Version 3.0 2023'</t>
+  </si>
+  <si>
+    <t>200 countries are included in the WIC Data Explorer. However, for 15 countries (Antigua and Barbuda, Barbados, Brunei Darussalem, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara), we did not find (good quality) education data. Hence, regional averages or similar countries were used instead and we recommend careful use of their data. World regions and sub regions are adopted from the United Nations (UN). For more information on the UN definitions click &lt;a href='https://unstats.un.org/unsd/methodology/m49/'&gt;here&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Due to methodological constraints, only countries with a population of more than 80,000 people in 2020 are currently considered in the database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The projection data come from population projections carried out by researchers at WIC. They are based on several data collection excercises for the base-year data and historical reconstruction to 1950. The research also uses largely the data produced by &lt;a href='http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm'&gt;World Population Prospects: The 2022 revision&lt;/a&gt; by the United Nations Population Division (2020 base-year population by age and sex and estimates for 1950-2020, and information about fertility, mortality and migration and related indicators for 1950-2020). The data are explained in several publications: KC et al. (2024), Yildiz and Abel (2024), Moradhvaj and KC (2024 forthcoming) and  Adhikari et al. (2024 forthcoming). The methodology and the rationale behind the assumptions underlying the scenarios are detailed in: &lt;a href='https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries'&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt; and &lt;a href='https://global.oup.com/academic/product/world-population-and-human-capital-in-the-twenty-first-century-9780198703167?cc=at&amp;lang=en'&gt;Lutz, Butz, and K.C. (Eds.) (2014)&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>For 15 countries it was not possible to obtain (good quality) data on educational attainment for the base year. Hence, approximations based on regional averages or similar countries were computed instead. Data for these countries should be used with utmost care. The countries in question are the following: Antigua and Barbuda, Barbados, Brunei Darussalem, Djibouti, Eritrea, Grenada, Guam, Libya, Mauritania, Mayotte, Papua New Guinea, Seychelles, United States Virgin Islands, Uzbekistan, and Western Sahara.</t>
+  </si>
+  <si>
+    <t>Education categories used in the projections are in line with selected UNESCO's &lt;a href='http://www.uis.unesco.org/Education/Pages/international-standard-classification-of-education.aspx'&gt;International Standard Classification of Education (ISCED 2011) categories&lt;/a&gt;. For details on WIC categories, see KC et al. (2024),  &lt;a href='https://www.oeaw.ac.at/fileadmin/subsites/Institute/VID/IMG/Publications/Working_Papers/WP2019_02.pdf'&gt;Speringer et al., 2019, VID WP 02/2019&lt;/a&gt; or the Education Definitions tab.</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1179,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,7 +1233,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1255,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1266,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1325,10 +1307,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1336,10 +1318,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,7 +1343,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,7 +1354,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1380,10 +1362,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -1394,7 +1376,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1416,7 +1398,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1424,10 +1406,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1435,10 +1417,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1446,10 +1428,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1457,10 +1439,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1468,54 +1450,54 @@
         <v>8</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>34</v>
+      <c r="B25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="4" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>48</v>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1523,10 +1505,10 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1534,10 +1516,10 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1545,10 +1527,10 @@
         <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1556,50 +1538,17 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
first update to v31
</commit_message>
<xml_diff>
--- a/meta/faq.xlsx
+++ b/meta/faq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yildiz\Dropbox\WIC Projections 2022\WCDE for Guy\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy Abel\Documents\Github\wcde-shiny\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8329B4C1-5B0D-4B05-BA4E-79114D9A9EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009596D-83F7-48EA-A853-E8B58D26A1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1110" windowWidth="26790" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="faq" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>category</t>
   </si>
@@ -290,12 +290,29 @@
   <si>
     <t xml:space="preserve">The projection data come from population projections carried out by researchers at WIC. They are based on several data collection excercises for the base-year data and historical reconstruction to 1950. The research also uses largely the data produced by &lt;a href='http://esa.un.org/wpp/documentation/WPP%202010%20publications.htm'&gt;World Population Prospects: The 2022 revision&lt;/a&gt; by the United Nations Population Division (2020 base-year population by age and sex and estimates for 1950-2020, and information about fertility, mortality and migration and related indicators for 1950-2020). The data are explained in several publications:  &lt;a href='https://pure.iiasa.ac.at/19487'&gt;K.C. et al. (2024)&lt;/a&gt;,  &lt;a href='https://pure.iiasa.ac.at/19399'&gt;Yildiz and Abel (2024)&lt;/a&gt;, Dhakad and KC (2024 forthcoming) and  Adhikari et al. (2024 forthcoming). The methodology and the rationale behind the assumptions underlying the scenarios are detailed in: &lt;a href='https://ec.europa.eu/jrc/en/publication/demographic-and-human-capital-scenarios-21st-century-2018-assessment-201-countries'&gt;Lutz, Goujon, KC, Stonawski, and Stilianakis (Eds.) (2018)&lt;/a&gt; and &lt;a href='https://global.oup.com/academic/product/world-population-and-human-capital-in-the-twenty-first-century-9780198703167?cc=at&amp;lang=en'&gt;Lutz, Butz, and K.C. (Eds.) (2014)&lt;/a&gt;. </t>
   </si>
+  <si>
+    <t>What is different in version 3.1</t>
+  </si>
+  <si>
+    <r>
+      <t>Due to a coding error, we noticed that the education data for men and women had been reversed in the base year for 37 countries listed below. As a result, we reran the projections and validated the outcomes, which led to minor changes in the population numbers for the affected countries. They are the following (with UN country code): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>32 Argentina, 44 Bahamas, 48 Bahrain, 64 Bhutan, 76 Brazil, 108 Burundi, 132 Cabo Verde, 156 China, 158 China, Taiwan Province of China, 170 Colombia, 214 Dominican Republic, 218 Ecuador, 226 Equatorial Guinea, 288 Ghana, 296 Kiribati, 360 Indonesia, 392 Japan, 400 Jordan, 410 Republic of Korea, 414 Kuwait, 496 Mongolia, 528 Netherlands, 558 Nicaragua, 583 Micronesia (Fed. States of), 591 Panama, 626 Timor-Leste, 630 Puerto Rico, 634 Qatar, 643 Russian Federation, 662 Saint Lucia, 702 Singapore, 764 Thailand, 784 United Arab Emirates, 788 Tunisia, 792 Turkey, 840 United States of America, 894 Zambia</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +462,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -788,12 +817,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1144,18 +1174,18 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="163.26953125" customWidth="1"/>
-    <col min="3" max="3" width="255.54296875" customWidth="1"/>
+    <col min="2" max="2" width="163.28515625" customWidth="1"/>
+    <col min="3" max="3" width="255.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1207,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1188,7 +1218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1229,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +1240,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +1251,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1232,7 +1262,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1243,7 +1273,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1284,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1265,7 +1295,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1276,7 +1306,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1317,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1309,7 +1339,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1320,7 +1350,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1331,7 +1361,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1372,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1353,7 +1383,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1394,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1375,7 +1405,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1397,7 +1427,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1408,7 +1438,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1419,7 +1449,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1441,7 +1471,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1482,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1463,7 +1493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1474,7 +1504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1485,7 +1515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1526,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1507,10 +1537,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
     </row>
   </sheetData>

</xml_diff>